<commit_message>
Archivos reporte final Mead
</commit_message>
<xml_diff>
--- a/2017-feb-mead.xlsx
+++ b/2017-feb-mead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Starcom\mead\2017\feb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\d\Mead &amp; Johnson\2017\feb\mead\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Data Stream</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>Facebook-Ads</t>
-  </si>
-  <si>
-    <t>Mead Johnson - 201702 - PPA 01  - Promo mi vasito y mi platito</t>
-  </si>
-  <si>
-    <t>20170203 - PPA - Promo mi vasito y mi platito</t>
   </si>
   <si>
     <t>PPA - Promo mi vasito y mi platito</t>
@@ -110,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -188,7 +182,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -197,7 +191,7 @@
     <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -479,28 +473,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,13 +508,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -541,59 +535,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3">
-        <v>933333.33333333337</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1462385</v>
+      <c r="E2" s="4">
+        <v>1541433.3333333335</v>
+      </c>
+      <c r="F2">
+        <v>2129003</v>
       </c>
       <c r="G2" s="4">
-        <v>18667</v>
-      </c>
-      <c r="H2" s="2">
-        <v>27528</v>
-      </c>
-      <c r="I2" s="2">
-        <v>20296</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1.0153272038571428</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1400.0000000000002</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1438786</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1.8824044283824028E-2</v>
+        <v>30829</v>
+      </c>
+      <c r="H2">
+        <v>41086</v>
+      </c>
+      <c r="I2">
+        <v>30308</v>
+      </c>
+      <c r="J2">
+        <v>1.0998781169285714</v>
+      </c>
+      <c r="K2">
+        <v>2311</v>
+      </c>
+      <c r="L2">
+        <v>1983574</v>
+      </c>
+      <c r="M2">
+        <v>1.9298234901500844E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="3">
         <v>563880</v>
@@ -623,18 +617,18 @@
         <v>1.4019200818524567E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="3">
         <v>566946.66666666663</v>
@@ -664,18 +658,18 @@
         <v>3.6147454587293147E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E5" s="3">
         <v>608100</v>
@@ -703,47 +697,6 @@
       </c>
       <c r="M5" s="2">
         <v>2.217882816912194E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3">
-        <v>608100</v>
-      </c>
-      <c r="F6" s="2">
-        <v>666618</v>
-      </c>
-      <c r="G6" s="3">
-        <v>12162</v>
-      </c>
-      <c r="H6" s="2">
-        <v>13558</v>
-      </c>
-      <c r="I6" s="2">
-        <v>10012</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1.18442903</v>
-      </c>
-      <c r="K6" s="2">
-        <v>911</v>
-      </c>
-      <c r="L6" s="2">
-        <v>544788</v>
-      </c>
-      <c r="M6" s="2">
-        <v>2.0338484709383785E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>